<commit_message>
fix error and add update for tbl_alumni
</commit_message>
<xml_diff>
--- a/tracer dikti.xlsx
+++ b/tracer dikti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="17220" windowHeight="7090"/>
+    <workbookView xWindow="480" yWindow="96" windowWidth="17220" windowHeight="7092"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,10 +15,197 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+  <si>
+    <t>f171</t>
+  </si>
+  <si>
+    <t>f175</t>
+  </si>
+  <si>
+    <t>f1743</t>
+  </si>
+  <si>
+    <t>f173</t>
+  </si>
+  <si>
+    <t>f175a</t>
+  </si>
+  <si>
+    <t>f177</t>
+  </si>
+  <si>
+    <t>f179</t>
+  </si>
+  <si>
+    <t>f1711</t>
+  </si>
+  <si>
+    <t>f1713</t>
+  </si>
+  <si>
+    <t>f1715</t>
+  </si>
+  <si>
+    <t>f1717</t>
+  </si>
+  <si>
+    <t>f1719</t>
+  </si>
+  <si>
+    <t>f1721</t>
+  </si>
+  <si>
+    <t>f1723</t>
+  </si>
+  <si>
+    <t>f1725</t>
+  </si>
+  <si>
+    <t>f1727</t>
+  </si>
+  <si>
+    <t>f1729</t>
+  </si>
+  <si>
+    <t>f1731</t>
+  </si>
+  <si>
+    <t>f1733</t>
+  </si>
+  <si>
+    <t>f1735</t>
+  </si>
+  <si>
+    <t>f1737</t>
+  </si>
+  <si>
+    <t>f1737a</t>
+  </si>
+  <si>
+    <t>f1739</t>
+  </si>
+  <si>
+    <t>f1741</t>
+  </si>
+  <si>
+    <t>f1745</t>
+  </si>
+  <si>
+    <t>f1747</t>
+  </si>
+  <si>
+    <t>f1749</t>
+  </si>
+  <si>
+    <t>f1751</t>
+  </si>
+  <si>
+    <t>f1753</t>
+  </si>
+  <si>
+    <t>f172b</t>
+  </si>
+  <si>
+    <t>f174b</t>
+  </si>
+  <si>
+    <t>f176b</t>
+  </si>
+  <si>
+    <t>f176ba</t>
+  </si>
+  <si>
+    <t>f178b</t>
+  </si>
+  <si>
+    <t>f1710b</t>
+  </si>
+  <si>
+    <t>f1712b</t>
+  </si>
+  <si>
+    <t>f1714b</t>
+  </si>
+  <si>
+    <t>f1716b</t>
+  </si>
+  <si>
+    <t>f1718b</t>
+  </si>
+  <si>
+    <t>f1720b</t>
+  </si>
+  <si>
+    <t>f1722b</t>
+  </si>
+  <si>
+    <t>f1724b</t>
+  </si>
+  <si>
+    <t>f1726b</t>
+  </si>
+  <si>
+    <t>f1728b</t>
+  </si>
+  <si>
+    <t>f1730b</t>
+  </si>
+  <si>
+    <t>f1732b</t>
+  </si>
+  <si>
+    <t>f1734b</t>
+  </si>
+  <si>
+    <t>f1736b</t>
+  </si>
+  <si>
+    <t>f1738b</t>
+  </si>
+  <si>
+    <t>f1738ba</t>
+  </si>
+  <si>
+    <t>f1740b</t>
+  </si>
+  <si>
+    <t>f1742b</t>
+  </si>
+  <si>
+    <t>f1744b</t>
+  </si>
+  <si>
+    <t>f1746b</t>
+  </si>
+  <si>
+    <t>f1748b</t>
+  </si>
+  <si>
+    <t>f1750b</t>
+  </si>
+  <si>
+    <t>f1752b</t>
+  </si>
+  <si>
+    <t>f1754b</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -46,8 +233,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -85,7 +278,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="12192627" cy="56978902"/>
+          <a:ext cx="12192627" cy="57405456"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="12065627" cy="58941052"/>
         </a:xfrm>
@@ -379,6 +572,63 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1997535" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="TextBox 15"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3893820" y="34792920"/>
+          <a:ext cx="1997535" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>JIKA</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> !== [1], maka lanjut ke f17</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -669,16 +919,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="U236:V264"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM279" sqref="AM279"/>
+    <sheetView tabSelected="1" topLeftCell="O245" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="V236" sqref="V236:V264"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="21" max="22" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="236" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U236" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V236" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="237" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U237" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V237" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="238" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U238" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V238" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="239" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U239" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V239" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="240" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U240" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="V240" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="241" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U241" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V241" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="242" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U242" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="V242" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="243" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U243" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V243" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="244" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U244" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V244" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="245" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U245" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="V245" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="246" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U246" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="V246" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="247" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U247" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="V247" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="248" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U248" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V248" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="249" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U249" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="V249" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="250" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U250" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="V250" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="251" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U251" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V251" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="252" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U252" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="V252" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="253" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U253" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V253" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="254" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U254" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V254" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="255" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U255" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V255" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="256" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U256" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V256" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="257" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U257" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V257" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="258" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U258" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="V258" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="259" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U259" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V259" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="260" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U260" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V260" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="261" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U261" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="V261" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="262" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U262" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V262" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="263" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U263" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="V263" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="264" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U264" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V264" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -688,7 +1175,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -700,7 +1187,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update backend tracer laporan
</commit_message>
<xml_diff>
--- a/tracer dikti.xlsx
+++ b/tracer dikti.xlsx
@@ -4,14 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="96" windowWidth="17220" windowHeight="7092"/>
+    <workbookView xWindow="480" yWindow="100" windowWidth="17220" windowHeight="7090"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$T$310</definedName>
+  </definedNames>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -278,7 +281,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="12192627" cy="57405456"/>
+          <a:ext cx="12277294" cy="55670802"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="12065627" cy="58941052"/>
         </a:xfrm>
@@ -921,16 +924,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="U236:V264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O245" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V236" sqref="V236:V264"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A225" zoomScale="60" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Z249" sqref="Z249"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="21" max="22" width="8.88671875" style="1"/>
+    <col min="21" max="22" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="236" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="236" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U236" s="2" t="s">
         <v>0</v>
       </c>
@@ -938,7 +941,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="237" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="237" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U237" s="2" t="s">
         <v>3</v>
       </c>
@@ -946,7 +949,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="238" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="238" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U238" s="2" t="s">
         <v>1</v>
       </c>
@@ -954,7 +957,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="239" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="239" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U239" s="2" t="s">
         <v>4</v>
       </c>
@@ -962,7 +965,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="240" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="240" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U240" s="2" t="s">
         <v>5</v>
       </c>
@@ -970,7 +973,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="241" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U241" s="2" t="s">
         <v>6</v>
       </c>
@@ -978,7 +981,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="242" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="242" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U242" s="2" t="s">
         <v>7</v>
       </c>
@@ -986,7 +989,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="243" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="243" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U243" s="2" t="s">
         <v>8</v>
       </c>
@@ -994,7 +997,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="244" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="244" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U244" s="2" t="s">
         <v>9</v>
       </c>
@@ -1002,7 +1005,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="245" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="245" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U245" s="2" t="s">
         <v>10</v>
       </c>
@@ -1010,7 +1013,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="246" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="246" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U246" s="2" t="s">
         <v>11</v>
       </c>
@@ -1018,7 +1021,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="247" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="247" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U247" s="2" t="s">
         <v>12</v>
       </c>
@@ -1026,7 +1029,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="248" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="248" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U248" s="2" t="s">
         <v>13</v>
       </c>
@@ -1034,7 +1037,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="249" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="249" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U249" s="2" t="s">
         <v>14</v>
       </c>
@@ -1042,7 +1045,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="250" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="250" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U250" s="2" t="s">
         <v>15</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="251" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="251" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U251" s="2" t="s">
         <v>16</v>
       </c>
@@ -1058,7 +1061,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="252" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="252" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U252" s="2" t="s">
         <v>17</v>
       </c>
@@ -1066,7 +1069,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="253" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="253" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U253" s="2" t="s">
         <v>18</v>
       </c>
@@ -1074,7 +1077,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="254" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="254" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U254" s="2" t="s">
         <v>19</v>
       </c>
@@ -1082,7 +1085,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="255" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="255" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U255" s="2" t="s">
         <v>20</v>
       </c>
@@ -1090,7 +1093,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="256" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="256" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U256" s="2" t="s">
         <v>21</v>
       </c>
@@ -1098,7 +1101,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="257" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="257" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U257" s="2" t="s">
         <v>22</v>
       </c>
@@ -1106,7 +1109,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="258" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="258" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U258" s="2" t="s">
         <v>23</v>
       </c>
@@ -1114,7 +1117,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="259" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="259" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U259" s="2" t="s">
         <v>2</v>
       </c>
@@ -1122,7 +1125,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="260" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="260" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U260" s="2" t="s">
         <v>24</v>
       </c>
@@ -1130,7 +1133,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="261" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="261" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U261" s="2" t="s">
         <v>25</v>
       </c>
@@ -1138,7 +1141,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="262" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="262" spans="21:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="U262" s="2" t="s">
         <v>26</v>
       </c>
@@ -1146,7 +1149,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="263" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="263" spans="21:22" x14ac:dyDescent="0.35">
       <c r="U263" s="2" t="s">
         <v>27</v>
       </c>
@@ -1154,7 +1157,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="264" spans="21:22" x14ac:dyDescent="0.3">
+    <row r="264" spans="21:22" x14ac:dyDescent="0.35">
       <c r="U264" s="2" t="s">
         <v>28</v>
       </c>
@@ -1164,7 +1167,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="70" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -1175,7 +1178,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1187,7 +1190,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>